<commit_message>
Matouqin: update data and readme.txt
</commit_message>
<xml_diff>
--- a/models/matouqin/Data/data_structure.xlsx
+++ b/models/matouqin/Data/data_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\model\yayue\models\matouqin\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E91B5FB-2668-47F6-B997-0D7675005918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2520FC-E735-4970-AB83-2160F45F8725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{AEEBE647-0CC9-4089-B5C6-ED9E548DECB5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="3" xr2:uid="{AEEBE647-0CC9-4089-B5C6-ED9E548DECB5}"/>
   </bookViews>
   <sheets>
     <sheet name="inflow-cf" sheetId="1" r:id="rId1"/>
@@ -1029,7 +1029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{242E8666-AD35-47D5-AF75-40A218378C62}">
   <dimension ref="A1:C8761"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -71219,8 +71219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA09C07B-97B6-4944-81CD-58D528438C11}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>